<commit_message>
teosinte genetic matrices added, selection test code included
</commit_message>
<xml_diff>
--- a/PhenotypeData/tmp_TeosintepopsAverage.xlsx
+++ b/PhenotypeData/tmp_TeosintepopsAverage.xlsx
@@ -907,8 +907,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1078,7 +1082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1161,6 +1165,8 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1243,6 +1249,8 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1574,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AS201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB172" workbookViewId="0">
-      <selection activeCell="AS201" sqref="B201:AS201"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>